<commit_message>
V2_2308_SIS_predoc_Climate change & sustainability
</commit_message>
<xml_diff>
--- a/Data/Dataset_environmental_sustainability.xlsx
+++ b/Data/Dataset_environmental_sustainability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinkettu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66b5d03f9f54eb73/Work/[C] Quantitative research methods/quant_rm/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAED25D0-6E67-B54A-99D4-046902AF580D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DAED25D0-6E67-B54A-99D4-046902AF580D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE3A8720-9D4B-42B2-AE87-01A87F5CDD6C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26320" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,7 +237,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -467,26 +467,26 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="3.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="28" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="33" width="21.5" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="14.5" style="2"/>
+    <col min="29" max="33" width="21.42578125" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -572,7 +572,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -658,7 +658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -744,7 +744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -830,7 +830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -916,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>51</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>51</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>50</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>50</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>50</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>50</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>50</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>50</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>50</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>50</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>50</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>50</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>50</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>50</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>50</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>50</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>50</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>50</v>
       </c>
@@ -6764,7 +6764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>50</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>50</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>50</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>50</v>
       </c>
@@ -7108,7 +7108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>50</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>50</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>50</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>50</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>50</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>50</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>50</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>50</v>
       </c>
@@ -7796,7 +7796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>50</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>50</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>50</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>50</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>50</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>50</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>50</v>
       </c>
@@ -8398,7 +8398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>50</v>
       </c>
@@ -8484,7 +8484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>50</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>50</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>50</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>50</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>50</v>
       </c>
@@ -8914,7 +8914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>50</v>
       </c>
@@ -9000,7 +9000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>50</v>
       </c>
@@ -9086,7 +9086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>50</v>
       </c>
@@ -9172,7 +9172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>50</v>
       </c>
@@ -9258,7 +9258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>50</v>
       </c>
@@ -9344,7 +9344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>50</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>50</v>
       </c>
@@ -9516,7 +9516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>50</v>
       </c>
@@ -9602,7 +9602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>50</v>
       </c>
@@ -9688,7 +9688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>50</v>
       </c>
@@ -9774,7 +9774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>50</v>
       </c>
@@ -9860,7 +9860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>50</v>
       </c>
@@ -9946,7 +9946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>50</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>50</v>
       </c>
@@ -10118,7 +10118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>50</v>
       </c>
@@ -10204,7 +10204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>50</v>
       </c>
@@ -10290,7 +10290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>50</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>50</v>
       </c>
@@ -10462,7 +10462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>50</v>
       </c>
@@ -10548,7 +10548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>50</v>
       </c>
@@ -10634,7 +10634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>50</v>
       </c>
@@ -10720,7 +10720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>50</v>
       </c>
@@ -10806,7 +10806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>50</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>50</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>50</v>
       </c>
@@ -11064,7 +11064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>50</v>
       </c>
@@ -11150,7 +11150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>50</v>
       </c>
@@ -11236,7 +11236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>50</v>
       </c>
@@ -11322,7 +11322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>50</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>50</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>50</v>
       </c>
@@ -11580,7 +11580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>50</v>
       </c>
@@ -11666,7 +11666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>50</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>50</v>
       </c>
@@ -11838,7 +11838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>50</v>
       </c>
@@ -11924,7 +11924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>50</v>
       </c>
@@ -12010,7 +12010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>50</v>
       </c>
@@ -12096,7 +12096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>50</v>
       </c>
@@ -12182,7 +12182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>50</v>
       </c>
@@ -12268,7 +12268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>50</v>
       </c>
@@ -12354,7 +12354,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>50</v>
       </c>
@@ -12440,7 +12440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>50</v>
       </c>
@@ -12526,7 +12526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>50</v>
       </c>
@@ -12612,7 +12612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>50</v>
       </c>
@@ -12698,7 +12698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>50</v>
       </c>
@@ -12784,7 +12784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>50</v>
       </c>
@@ -12870,7 +12870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>50</v>
       </c>
@@ -12956,7 +12956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>50</v>
       </c>
@@ -13042,7 +13042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>50</v>
       </c>
@@ -13128,7 +13128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>50</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>50</v>
       </c>
@@ -13300,7 +13300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>50</v>
       </c>
@@ -13386,7 +13386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>50</v>
       </c>
@@ -13472,7 +13472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>50</v>
       </c>
@@ -13558,7 +13558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>50</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>50</v>
       </c>
@@ -13730,7 +13730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>50</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>50</v>
       </c>
@@ -13902,7 +13902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>50</v>
       </c>
@@ -13988,7 +13988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>50</v>
       </c>
@@ -14074,7 +14074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>50</v>
       </c>
@@ -14160,7 +14160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>50</v>
       </c>
@@ -14246,7 +14246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>50</v>
       </c>
@@ -14332,7 +14332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>50</v>
       </c>
@@ -14418,7 +14418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>50</v>
       </c>
@@ -14504,7 +14504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>50</v>
       </c>
@@ -14590,7 +14590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>50</v>
       </c>
@@ -14676,7 +14676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>50</v>
       </c>
@@ -14762,7 +14762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>50</v>
       </c>
@@ -14848,7 +14848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>50</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>50</v>
       </c>
@@ -15020,7 +15020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>50</v>
       </c>
@@ -15106,7 +15106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>50</v>
       </c>
@@ -15192,7 +15192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>50</v>
       </c>
@@ -15278,7 +15278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>50</v>
       </c>
@@ -15364,7 +15364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>50</v>
       </c>
@@ -15450,7 +15450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>50</v>
       </c>
@@ -15536,7 +15536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>50</v>
       </c>
@@ -15622,7 +15622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>50</v>
       </c>
@@ -15708,7 +15708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>50</v>
       </c>
@@ -15794,7 +15794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>50</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>50</v>
       </c>
@@ -15966,7 +15966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>50</v>
       </c>
@@ -16052,7 +16052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>50</v>
       </c>
@@ -16138,7 +16138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>50</v>
       </c>
@@ -16224,7 +16224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>50</v>
       </c>
@@ -16310,7 +16310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>50</v>
       </c>
@@ -16396,7 +16396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>50</v>
       </c>
@@ -16482,7 +16482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>50</v>
       </c>
@@ -16568,7 +16568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>50</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>50</v>
       </c>
@@ -16740,7 +16740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>50</v>
       </c>
@@ -16826,7 +16826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>50</v>
       </c>
@@ -16912,7 +16912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>50</v>
       </c>
@@ -16998,7 +16998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>50</v>
       </c>
@@ -17084,7 +17084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>50</v>
       </c>
@@ -17170,7 +17170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>50</v>
       </c>
@@ -17256,7 +17256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>50</v>
       </c>
@@ -17342,7 +17342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>51</v>
       </c>
@@ -17428,7 +17428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>50</v>
       </c>
@@ -17514,7 +17514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>50</v>
       </c>
@@ -17600,7 +17600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>50</v>
       </c>
@@ -17686,7 +17686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>50</v>
       </c>
@@ -17772,7 +17772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>50</v>
       </c>
@@ -17858,7 +17858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>50</v>
       </c>
@@ -17944,7 +17944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>50</v>
       </c>
@@ -18030,7 +18030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>50</v>
       </c>
@@ -18116,7 +18116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>50</v>
       </c>
@@ -18202,7 +18202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>50</v>
       </c>
@@ -18288,7 +18288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>50</v>
       </c>
@@ -18374,7 +18374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>50</v>
       </c>
@@ -18460,7 +18460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>50</v>
       </c>
@@ -18546,7 +18546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>50</v>
       </c>
@@ -18632,7 +18632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="212" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>50</v>
       </c>
@@ -18718,7 +18718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>50</v>
       </c>
@@ -18804,7 +18804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>50</v>
       </c>
@@ -18890,7 +18890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>50</v>
       </c>
@@ -18976,7 +18976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>50</v>
       </c>
@@ -19062,7 +19062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="217" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>50</v>
       </c>
@@ -19148,7 +19148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>50</v>
       </c>
@@ -19234,7 +19234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>50</v>
       </c>
@@ -19320,7 +19320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>50</v>
       </c>
@@ -19406,7 +19406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="221" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>50</v>
       </c>
@@ -19492,7 +19492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>50</v>
       </c>
@@ -19578,7 +19578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>50</v>
       </c>
@@ -19664,7 +19664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="224" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>50</v>
       </c>
@@ -19750,7 +19750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="225" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>50</v>
       </c>
@@ -19836,7 +19836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>50</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>50</v>
       </c>
@@ -20008,7 +20008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>50</v>
       </c>
@@ -20094,7 +20094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>50</v>
       </c>
@@ -20180,7 +20180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>50</v>
       </c>
@@ -20266,7 +20266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>50</v>
       </c>
@@ -20352,7 +20352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>50</v>
       </c>
@@ -20438,7 +20438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>50</v>
       </c>
@@ -20524,7 +20524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>50</v>
       </c>
@@ -20610,7 +20610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>50</v>
       </c>
@@ -20696,7 +20696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>50</v>
       </c>
@@ -20782,7 +20782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="237" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>50</v>
       </c>
@@ -20868,7 +20868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>50</v>
       </c>
@@ -20954,7 +20954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>50</v>
       </c>
@@ -21040,7 +21040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>50</v>
       </c>
@@ -21126,7 +21126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>50</v>
       </c>
@@ -21212,7 +21212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>50</v>
       </c>
@@ -21298,7 +21298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="243" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>50</v>
       </c>
@@ -21384,7 +21384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="244" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>50</v>
       </c>
@@ -21470,7 +21470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>50</v>
       </c>
@@ -21556,7 +21556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>50</v>
       </c>
@@ -21642,7 +21642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="247" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>50</v>
       </c>
@@ -21728,7 +21728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>50</v>
       </c>
@@ -21814,7 +21814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>50</v>
       </c>
@@ -21900,7 +21900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="250" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>50</v>
       </c>
@@ -21986,7 +21986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="251" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>50</v>
       </c>
@@ -22072,7 +22072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>50</v>
       </c>
@@ -22158,7 +22158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>50</v>
       </c>
@@ -22244,7 +22244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="254" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>50</v>
       </c>
@@ -22330,7 +22330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>50</v>
       </c>
@@ -22416,7 +22416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="256" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>50</v>
       </c>
@@ -22502,7 +22502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>50</v>
       </c>
@@ -22588,7 +22588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="258" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>50</v>
       </c>
@@ -22674,7 +22674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>50</v>
       </c>
@@ -22760,7 +22760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="260" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>50</v>
       </c>
@@ -22846,7 +22846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="261" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>50</v>
       </c>
@@ -22932,7 +22932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>50</v>
       </c>
@@ -23018,7 +23018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>50</v>
       </c>
@@ -23104,7 +23104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>50</v>
       </c>
@@ -23190,7 +23190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>50</v>
       </c>
@@ -23276,7 +23276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="266" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>50</v>
       </c>
@@ -23362,7 +23362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="267" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>50</v>
       </c>
@@ -23448,7 +23448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>50</v>
       </c>
@@ -23534,7 +23534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="269" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>50</v>
       </c>
@@ -23620,7 +23620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>50</v>
       </c>
@@ -23706,7 +23706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>50</v>
       </c>
@@ -23792,7 +23792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>50</v>
       </c>
@@ -23878,7 +23878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>50</v>
       </c>
@@ -23964,7 +23964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>50</v>
       </c>
@@ -24050,7 +24050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="275" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>50</v>
       </c>
@@ -24136,7 +24136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>50</v>
       </c>
@@ -24222,7 +24222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="277" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
         <v>50</v>
       </c>
@@ -24308,7 +24308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="278" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>50</v>
       </c>
@@ -24394,7 +24394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
         <v>50</v>
       </c>
@@ -24480,7 +24480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>50</v>
       </c>
@@ -24566,7 +24566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="281" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>50</v>
       </c>
@@ -24652,7 +24652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>50</v>
       </c>
@@ -24738,7 +24738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>50</v>
       </c>
@@ -24824,7 +24824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>50</v>
       </c>
@@ -24910,7 +24910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>50</v>
       </c>
@@ -24996,7 +24996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>50</v>
       </c>
@@ -25082,7 +25082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>50</v>
       </c>
@@ -25168,7 +25168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>50</v>
       </c>
@@ -25254,7 +25254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="289" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>50</v>
       </c>
@@ -25340,7 +25340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="290" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>50</v>
       </c>
@@ -25426,7 +25426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
         <v>50</v>
       </c>
@@ -25512,7 +25512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="292" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>50</v>
       </c>
@@ -25598,7 +25598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
         <v>50</v>
       </c>
@@ -25684,7 +25684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>50</v>
       </c>
@@ -25770,7 +25770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
         <v>50</v>
       </c>
@@ -25856,7 +25856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="296" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>50</v>
       </c>
@@ -25942,7 +25942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
         <v>50</v>
       </c>
@@ -26028,7 +26028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>50</v>
       </c>
@@ -26114,7 +26114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>50</v>
       </c>
@@ -26200,7 +26200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="300" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>50</v>
       </c>
@@ -26286,7 +26286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="301" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>50</v>
       </c>
@@ -26372,7 +26372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="302" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>50</v>
       </c>
@@ -26458,7 +26458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
         <v>50</v>
       </c>
@@ -26544,7 +26544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="304" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>50</v>
       </c>
@@ -26630,7 +26630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="305" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>50</v>
       </c>
@@ -26716,7 +26716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>50</v>
       </c>
@@ -26802,7 +26802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="307" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>50</v>
       </c>
@@ -26888,7 +26888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>50</v>
       </c>
@@ -26974,7 +26974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="309" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
         <v>50</v>
       </c>
@@ -27060,7 +27060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="310" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>50</v>
       </c>
@@ -27146,7 +27146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="311" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
         <v>50</v>
       </c>
@@ -27232,7 +27232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="312" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>50</v>
       </c>
@@ -27318,7 +27318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="313" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>